<commit_message>
Updated with some added instructions, we need to test it using the simulator, one step at a time and see the issue
</commit_message>
<xml_diff>
--- a/ListOfInstructions.xlsx
+++ b/ListOfInstructions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Coding\MIPS Coursework\arch2-2017-cw-SeanTheScot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\arch2-2017-cw-SeanTheScot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16400" windowHeight="8190" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
   <si>
     <t>Instructions</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -478,11 +481,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFE2E5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -498,6 +510,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -882,21 +900,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375"/>
-    <col min="2" max="2" width="22.7109375"/>
+    <col min="1" max="1" width="10.7265625"/>
+    <col min="2" max="2" width="22.7265625"/>
     <col min="3" max="3" width="12"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625"/>
-    <col min="8" max="1026" width="8.5703125"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875"/>
+    <col min="8" max="1026" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -931,7 +949,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -943,7 +961,7 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -954,6 +972,9 @@
         <v>8</v>
       </c>
       <c r="D4" s="4"/>
+      <c r="E4" s="9" t="s">
+        <v>118</v>
+      </c>
       <c r="F4" t="s">
         <v>117</v>
       </c>
@@ -961,7 +982,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -972,8 +993,11 @@
         <v>15</v>
       </c>
       <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -984,8 +1008,11 @@
         <v>15</v>
       </c>
       <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -997,7 +1024,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +1036,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1022,7 +1049,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="23" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1062,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -1048,7 +1075,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="23" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1061,7 +1088,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1101,7 @@
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -1087,7 +1114,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1100,7 +1127,7 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1140,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -1126,7 +1153,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1139,7 +1166,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1152,7 +1179,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1165,7 +1192,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -1178,7 +1205,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1191,7 +1218,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -1204,7 +1231,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>54</v>
       </c>
@@ -1217,7 +1244,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
@@ -1230,7 +1257,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
@@ -1243,7 +1270,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
@@ -1256,7 +1283,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
@@ -1269,7 +1296,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>65</v>
       </c>
@@ -1282,7 +1309,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1295,7 +1322,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>69</v>
       </c>
@@ -1308,7 +1335,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -1321,7 +1348,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>73</v>
       </c>
@@ -1334,7 +1361,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>75</v>
       </c>
@@ -1345,9 +1372,11 @@
         <v>27</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>77</v>
       </c>
@@ -1358,9 +1387,11 @@
         <v>27</v>
       </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
@@ -1371,9 +1402,11 @@
         <v>15</v>
       </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>81</v>
       </c>
@@ -1386,7 +1419,7 @@
       <c r="D37" s="4"/>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
@@ -1399,7 +1432,7 @@
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>85</v>
       </c>
@@ -1412,7 +1445,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
@@ -1425,7 +1458,7 @@
       <c r="D40" s="4"/>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>89</v>
       </c>
@@ -1438,7 +1471,7 @@
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>91</v>
       </c>
@@ -1449,9 +1482,11 @@
         <v>8</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="E42" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>93</v>
       </c>
@@ -1462,9 +1497,11 @@
         <v>22</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="E43" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>95</v>
       </c>
@@ -1475,9 +1512,11 @@
         <v>22</v>
       </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>97</v>
       </c>
@@ -1488,9 +1527,11 @@
         <v>15</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>99</v>
       </c>
@@ -1503,7 +1544,7 @@
       <c r="D46" s="4"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>101</v>
       </c>
@@ -1516,7 +1557,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>102</v>
       </c>
@@ -1529,7 +1570,7 @@
       <c r="D48" s="6"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -1542,7 +1583,7 @@
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>106</v>
       </c>
@@ -1553,9 +1594,11 @@
         <v>8</v>
       </c>
       <c r="D50" s="6"/>
-      <c r="E50" s="7"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
@@ -1566,9 +1609,11 @@
         <v>15</v>
       </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
@@ -1581,7 +1626,7 @@
       <c r="D52" s="6"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
@@ -1592,9 +1637,11 @@
         <v>15</v>
       </c>
       <c r="D53" s="4"/>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="E53" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>114</v>
       </c>
@@ -1605,7 +1652,9 @@
         <v>8</v>
       </c>
       <c r="D54" s="4"/>
-      <c r="E54" s="7"/>
+      <c r="E54" s="9" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>